<commit_message>
Signed-off-by: 七国军队 <1211412423@qq.com> 秦辉
</commit_message>
<xml_diff>
--- a/doc/会议纪要/会议纪要.xlsx
+++ b/doc/会议纪要/会议纪要.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19830" windowHeight="9990" activeTab="1"/>
+    <workbookView windowWidth="19830" windowHeight="9990" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="封面" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,14 @@
     <sheet name="会议纪要7月12日" sheetId="7" r:id="rId7"/>
     <sheet name="会议纪要7月13日" sheetId="8" r:id="rId8"/>
     <sheet name="会议纪要7月14日" sheetId="9" r:id="rId9"/>
+    <sheet name="会议纪要7月15日" sheetId="10" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
     <externalReference r:id="rId12"/>
     <externalReference r:id="rId13"/>
     <externalReference r:id="rId14"/>
+    <externalReference r:id="rId15"/>
   </externalReferences>
   <definedNames>
     <definedName name="_ML1">[1]分类数据!$C$3</definedName>
@@ -343,8 +344,46 @@
 </comments>
 </file>
 
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>caowei</author>
+  </authors>
+  <commentList>
+    <comment ref="H10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">记录人负责记录会议议题讨论的结论：
+通过、不通过、完善后通过，延后讨论</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">记录人负责对会议决议进行跟踪，并标识跟踪状态：
+已解决、转入问题日志、接受改善建议</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154">
   <si>
     <t>密级：秘密</t>
   </si>
@@ -437,6 +476,12 @@
   </si>
   <si>
     <t>2014.7.14</t>
+  </si>
+  <si>
+    <t>v8.0</t>
+  </si>
+  <si>
+    <t>2014.7.15</t>
   </si>
   <si>
     <t>项目描述</t>
@@ -809,21 +854,51 @@
   <si>
     <t>将界面修改成JSP界面并设计数据统计界面</t>
   </si>
+  <si>
+    <t>对之前阶段总结</t>
+  </si>
+  <si>
+    <t>讨论下一阶段的实施方案</t>
+  </si>
+  <si>
+    <t>进行分工</t>
+  </si>
+  <si>
+    <t>简短讨论，再次分工</t>
+  </si>
+  <si>
+    <t>配置struts 2 pakage 和页面链接（客户管理，用户管理）</t>
+  </si>
+  <si>
+    <t>配置struts 2 pakage 和页面链接（统计报表，基础数据）</t>
+  </si>
+  <si>
+    <t>配置struts 2 pakage 和页面链接（营销管理，服务管理）</t>
+  </si>
+  <si>
+    <t>修改页面</t>
+  </si>
+  <si>
+    <t>检查、测试网站页面</t>
+  </si>
+  <si>
+    <t>修改文档</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="9">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="mmm"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;\&quot;* #,##0_);_(&quot;\&quot;* \(#,##0\);_(&quot;\&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="_(&quot;\&quot;* #,##0_);_(&quot;\&quot;* \(#,##0\);_(&quot;\&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;\&quot;* #,##0_);_(&quot;\&quot;* \(#,##0\);_(&quot;\&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="mmm"/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="180" formatCode="_(&quot;\&quot;* #,##0_);_(&quot;\&quot;* \(#,##0\);_(&quot;\&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -969,13 +1044,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="38"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
       <family val="38"/>
@@ -989,26 +1057,8 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="MS Sans Serif"/>
-      <family val="38"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="22"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="38"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="黑体"/>
-      <family val="54"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1025,6 +1075,39 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="MS Sans Serif"/>
+      <family val="38"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="38"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color indexed="12"/>
+      <name val="宋体"/>
+      <family val="7"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="黑体"/>
+      <family val="54"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="38"/>
+      <charset val="128"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color indexed="36"/>
@@ -1036,14 +1119,6 @@
       <u/>
       <sz val="12"/>
       <color indexed="20"/>
-      <name val="宋体"/>
-      <family val="7"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color indexed="12"/>
       <name val="宋体"/>
       <family val="7"/>
       <charset val="134"/>
@@ -1160,92 +1235,92 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="27" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="4">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="25" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1376,16 +1451,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="26" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="19" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="19" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="19" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="19" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1400,7 +1475,7 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="19" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="21" applyAlignment="1">
@@ -1445,10 +1520,10 @@
   </cellXfs>
   <cellStyles count="31">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="New Times Roman" xfId="1"/>
-    <cellStyle name="千位分隔" xfId="2" builtinId="3"/>
-    <cellStyle name="桁区切り [0.00]_(D)日程計画" xfId="3"/>
-    <cellStyle name="ColLevel_0" xfId="4"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="桁区切り [0.00]_(D)日程計画" xfId="2"/>
+    <cellStyle name="ColLevel_0" xfId="3"/>
+    <cellStyle name="New Times Roman" xfId="4"/>
     <cellStyle name="RowLevel_0" xfId="5"/>
     <cellStyle name="货币" xfId="6" builtinId="4"/>
     <cellStyle name="千位分隔[0]" xfId="7" builtinId="6"/>
@@ -1462,8 +1537,8 @@
     <cellStyle name="Normal_#10-Headcount" xfId="15"/>
     <cellStyle name="標準_(D)日程計画" xfId="16"/>
     <cellStyle name="表示済みのハイパーリンク_02_1st_2ndOTP対応機能一覧_一応完成版" xfId="17"/>
-    <cellStyle name="常规_G-OT0122 Rule or Guideline Template" xfId="18"/>
-    <cellStyle name="段落标题1" xfId="19"/>
+    <cellStyle name="段落标题1" xfId="18"/>
+    <cellStyle name="常规_G-OT0122 Rule or Guideline Template" xfId="19"/>
     <cellStyle name="常规_NSFT-PT029-软件开发计划模板" xfId="20"/>
     <cellStyle name="常规_封页" xfId="21"/>
     <cellStyle name="超链接" xfId="22" builtinId="8"/>
@@ -1471,8 +1546,8 @@
     <cellStyle name="访问过的超链接" xfId="24"/>
     <cellStyle name="桁区切り_(D)日程計画" xfId="25"/>
     <cellStyle name="普通" xfId="26"/>
-    <cellStyle name="千位[0]_laroux" xfId="27"/>
-    <cellStyle name="千位_laroux" xfId="28"/>
+    <cellStyle name="千位_laroux" xfId="27"/>
+    <cellStyle name="千位[0]_laroux" xfId="28"/>
     <cellStyle name="通貨 [0.00]_(D)日程計画" xfId="29"/>
     <cellStyle name="通貨_(D)日程計画" xfId="30"/>
   </cellStyles>
@@ -2313,13 +2388,497 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:H27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
+  <sheetData>
+    <row r="1" ht="27" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14">
+        <v>41835</v>
+      </c>
+      <c r="H6" s="15"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="19">
+        <v>1</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="19">
+        <v>2</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="19">
+        <v>3</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="19">
+        <v>4</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="19">
+        <v>5</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="23"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="19">
+        <v>6</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="23"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="19">
+        <v>7</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="25"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="19">
+        <v>8</v>
+      </c>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="25"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="19">
+        <v>9</v>
+      </c>
+      <c r="B19" s="26"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="25"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="29">
+        <v>1</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="29">
+        <v>2</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H22" s="34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="29">
+        <v>3</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" s="34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="29">
+        <v>4</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="H24" s="34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="29">
+        <v>5</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="29">
+        <v>6</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="29">
+        <v>7</v>
+      </c>
+      <c r="B27" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="H27" s="33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="39">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H11:H19">
+      <formula1>"通过,不通过,完善后通过,延后讨论"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H21:H27">
+      <formula1>"已解决,转入问题日志,接受改善建议"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="B1:I21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2525,7 +3084,25 @@
       </c>
       <c r="H11" s="46"/>
     </row>
-    <row r="12" ht="30" customHeight="1"/>
+    <row r="12" ht="30" customHeight="1" spans="2:8">
+      <c r="B12" s="46">
+        <v>9</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="46"/>
+    </row>
     <row r="13" ht="30" customHeight="1"/>
     <row r="14" ht="30" customHeight="1"/>
     <row r="15" ht="30" customHeight="1"/>
@@ -2540,7 +3117,7 @@
     <mergeCell ref="B1:H1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G8 G9:G11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G12 G4:G8 G9:G11">
       <formula1>"新建,增加,修改,删除"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2587,7 +3164,7 @@
     </row>
     <row r="3" ht="16.75" customHeight="1" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2599,33 +3176,33 @@
     </row>
     <row r="4" ht="16.75" customHeight="1" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H4" s="6"/>
     </row>
     <row r="5" ht="16.75" customHeight="1" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="7" t="s">
@@ -2635,7 +3212,7 @@
     </row>
     <row r="6" ht="16.75" customHeight="1" spans="1:8">
       <c r="A6" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2647,15 +3224,15 @@
     </row>
     <row r="7" ht="16.75" customHeight="1" spans="1:8">
       <c r="A7" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="14">
@@ -2665,15 +3242,15 @@
     </row>
     <row r="8" ht="16.75" customHeight="1" spans="1:8">
       <c r="A8" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="16" t="s">
@@ -2683,7 +3260,7 @@
     </row>
     <row r="9" ht="16.75" customHeight="1" spans="1:8">
       <c r="A9" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>18</v>
@@ -2697,10 +3274,10 @@
     </row>
     <row r="10" ht="16.75" customHeight="1" spans="1:8">
       <c r="A10" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -2711,7 +3288,7 @@
     </row>
     <row r="11" ht="20" customHeight="1" spans="1:8">
       <c r="A11" s="17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -2720,7 +3297,7 @@
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
       <c r="H11" s="18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1" spans="1:8">
@@ -2728,7 +3305,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
@@ -2736,7 +3313,7 @@
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
       <c r="H12" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1" spans="1:8">
@@ -2744,7 +3321,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
@@ -2752,7 +3329,7 @@
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
       <c r="H13" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1" spans="1:8">
@@ -2760,7 +3337,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -2768,7 +3345,7 @@
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
       <c r="H14" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1" spans="1:8">
@@ -2776,7 +3353,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
@@ -2784,7 +3361,7 @@
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
       <c r="H15" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1" spans="1:8">
@@ -2792,7 +3369,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="21"/>
@@ -2800,7 +3377,7 @@
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
       <c r="H16" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1" spans="1:8">
@@ -2808,7 +3385,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
@@ -2816,7 +3393,7 @@
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
       <c r="H17" s="25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1" spans="1:8">
@@ -2857,7 +3434,7 @@
     </row>
     <row r="21" ht="20" customHeight="1" spans="1:8">
       <c r="A21" s="17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -2865,10 +3442,10 @@
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
       <c r="G21" s="17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1" spans="1:8">
@@ -2876,7 +3453,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="30"/>
@@ -2886,7 +3463,7 @@
         <v>14</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1" spans="1:8">
@@ -2897,7 +3474,7 @@
       <c r="E23" s="30"/>
       <c r="F23" s="31"/>
       <c r="G23" s="32" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H23" s="25"/>
     </row>
@@ -2909,7 +3486,7 @@
       <c r="E24" s="30"/>
       <c r="F24" s="31"/>
       <c r="G24" s="32" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H24" s="25"/>
     </row>
@@ -2918,17 +3495,17 @@
         <v>2</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C25" s="29"/>
       <c r="D25" s="29"/>
       <c r="E25" s="29"/>
       <c r="F25" s="29"/>
       <c r="G25" s="32" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H25" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1" spans="1:8">
@@ -2936,17 +3513,17 @@
         <v>5</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C26" s="29"/>
       <c r="D26" s="29"/>
       <c r="E26" s="29"/>
       <c r="F26" s="29"/>
       <c r="G26" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H26" s="33" t="s">
         <v>70</v>
-      </c>
-      <c r="H26" s="33" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1" spans="1:8">
@@ -2954,17 +3531,17 @@
         <v>6</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
       <c r="F27" s="29"/>
       <c r="G27" s="32" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H27" s="33" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1" spans="1:8">
@@ -2972,17 +3549,17 @@
         <v>7</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C28" s="29"/>
       <c r="D28" s="29"/>
       <c r="E28" s="29"/>
       <c r="F28" s="29"/>
       <c r="G28" s="32" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H28" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1" spans="1:8">
@@ -2990,7 +3567,7 @@
         <v>8</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C29" s="29"/>
       <c r="D29" s="29"/>
@@ -3000,7 +3577,7 @@
         <v>18</v>
       </c>
       <c r="H29" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -3089,7 +3666,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3104,19 +3681,19 @@
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:11">
       <c r="A3" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="39"/>
@@ -3125,15 +3702,15 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="7" t="s">
@@ -3146,7 +3723,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -3161,15 +3738,15 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="11"/>
       <c r="E6" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="14">
@@ -3182,15 +3759,15 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="16" t="s">
@@ -3203,7 +3780,7 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>18</v>
@@ -3220,10 +3797,10 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -3237,7 +3814,7 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -3246,7 +3823,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I10" s="39"/>
       <c r="J10" s="39"/>
@@ -3257,7 +3834,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
@@ -3265,7 +3842,7 @@
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
       <c r="H11" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I11" s="39"/>
       <c r="J11" s="39"/>
@@ -3276,7 +3853,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
@@ -3284,7 +3861,7 @@
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
       <c r="H12" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I12" s="39"/>
       <c r="J12" s="39"/>
@@ -3295,7 +3872,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
@@ -3303,7 +3880,7 @@
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
       <c r="H13" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I13" s="39"/>
       <c r="J13" s="39"/>
@@ -3401,7 +3978,7 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -3409,10 +3986,10 @@
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I20" s="39"/>
       <c r="J20" s="39"/>
@@ -3423,7 +4000,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
@@ -3433,7 +4010,7 @@
         <v>14</v>
       </c>
       <c r="H21" s="33" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I21" s="39"/>
       <c r="J21" s="39"/>
@@ -3444,17 +4021,17 @@
         <v>2</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="30"/>
       <c r="E22" s="30"/>
       <c r="F22" s="31"/>
       <c r="G22" s="32" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H22" s="33" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I22" s="39"/>
       <c r="J22" s="39"/>
@@ -3465,17 +4042,17 @@
         <v>3</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
       <c r="F23" s="22"/>
       <c r="G23" s="32" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H23" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I23" s="39"/>
       <c r="J23" s="39"/>
@@ -3486,17 +4063,17 @@
         <v>4</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
       <c r="F24" s="22"/>
       <c r="G24" s="32" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H24" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I24" s="39"/>
       <c r="J24" s="39"/>
@@ -3507,7 +4084,7 @@
         <v>5</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
@@ -3517,7 +4094,7 @@
         <v>18</v>
       </c>
       <c r="H25" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I25" s="39"/>
       <c r="J25" s="39"/>
@@ -3528,17 +4105,17 @@
         <v>6</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
       <c r="F26" s="22"/>
       <c r="G26" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H26" s="33" t="s">
         <v>70</v>
-      </c>
-      <c r="H26" s="33" t="s">
-        <v>68</v>
       </c>
       <c r="I26" s="39"/>
       <c r="J26" s="39"/>
@@ -3549,17 +4126,17 @@
         <v>7</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
       <c r="F27" s="29"/>
       <c r="G27" s="32" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H27" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I27" s="39"/>
       <c r="J27" s="39"/>
@@ -3570,17 +4147,17 @@
         <v>8</v>
       </c>
       <c r="B28" s="38" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C28" s="36"/>
       <c r="D28" s="36"/>
       <c r="E28" s="36"/>
       <c r="F28" s="37"/>
       <c r="G28" s="32" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H28" s="33" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I28" s="39"/>
       <c r="J28" s="39"/>
@@ -3669,7 +4246,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3681,33 +4258,33 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="7" t="s">
@@ -3717,7 +4294,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -3729,15 +4306,15 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="11"/>
       <c r="E6" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="14">
@@ -3747,15 +4324,15 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="16" t="s">
@@ -3765,7 +4342,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>18</v>
@@ -3779,10 +4356,10 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -3793,7 +4370,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -3802,7 +4379,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -3810,7 +4387,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
@@ -3818,7 +4395,7 @@
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
       <c r="H11" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -3826,7 +4403,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
@@ -3834,7 +4411,7 @@
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
       <c r="H12" s="25" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -3842,7 +4419,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
@@ -3850,7 +4427,7 @@
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
       <c r="H13" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -3858,7 +4435,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -3866,7 +4443,7 @@
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
       <c r="H14" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -3874,7 +4451,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
@@ -3882,7 +4459,7 @@
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
       <c r="H15" s="25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -3890,7 +4467,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="21"/>
@@ -3898,7 +4475,7 @@
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
       <c r="H16" s="25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -3906,7 +4483,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
@@ -3914,7 +4491,7 @@
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
       <c r="H17" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -3943,7 +4520,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -3951,10 +4528,10 @@
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" ht="24" spans="1:8">
@@ -3962,17 +4539,17 @@
         <v>1</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
       <c r="E21" s="30"/>
       <c r="F21" s="31"/>
       <c r="G21" s="32" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H21" s="33" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" ht="24" spans="1:8">
@@ -3980,7 +4557,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="30"/>
@@ -3990,7 +4567,7 @@
         <v>14</v>
       </c>
       <c r="H22" s="33" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" ht="24" spans="1:8">
@@ -3998,17 +4575,17 @@
         <v>3</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
       <c r="F23" s="22"/>
       <c r="G23" s="32" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H23" s="33" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -4016,17 +4593,17 @@
         <v>4</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
       <c r="F24" s="22"/>
       <c r="G24" s="32" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H24" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" ht="24" spans="1:8">
@@ -4034,17 +4611,17 @@
         <v>5</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
       <c r="F25" s="22"/>
       <c r="G25" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25" s="33" t="s">
         <v>65</v>
-      </c>
-      <c r="H25" s="33" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -4052,17 +4629,17 @@
         <v>6</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
       <c r="F26" s="22"/>
       <c r="G26" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H26" s="33" t="s">
         <v>70</v>
-      </c>
-      <c r="H26" s="33" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -4070,17 +4647,17 @@
         <v>7</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
       <c r="F27" s="29"/>
       <c r="G27" s="32" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H27" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" ht="24" spans="1:8">
@@ -4088,7 +4665,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="38" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C28" s="36"/>
       <c r="D28" s="36"/>
@@ -4098,7 +4675,7 @@
         <v>18</v>
       </c>
       <c r="H28" s="33" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -4184,7 +4761,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4196,33 +4773,33 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="7" t="s">
@@ -4232,7 +4809,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -4244,15 +4821,15 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="11"/>
       <c r="E6" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="14">
@@ -4262,15 +4839,15 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="16" t="s">
@@ -4280,7 +4857,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>18</v>
@@ -4294,10 +4871,10 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -4308,7 +4885,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -4317,7 +4894,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -4325,7 +4902,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
@@ -4333,7 +4910,7 @@
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
       <c r="H11" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -4341,7 +4918,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
@@ -4349,7 +4926,7 @@
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
       <c r="H12" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -4357,7 +4934,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
@@ -4365,7 +4942,7 @@
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
       <c r="H13" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -4373,7 +4950,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -4381,7 +4958,7 @@
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
       <c r="H14" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -4389,7 +4966,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
@@ -4397,7 +4974,7 @@
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
       <c r="H15" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -4450,7 +5027,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -4458,10 +5035,10 @@
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -4469,17 +5046,17 @@
         <v>1</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
       <c r="E21" s="30"/>
       <c r="F21" s="31"/>
       <c r="G21" s="32" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H21" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -4487,17 +5064,17 @@
         <v>2</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="30"/>
       <c r="E22" s="30"/>
       <c r="F22" s="31"/>
       <c r="G22" s="32" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H22" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -4505,17 +5082,17 @@
         <v>3</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
       <c r="F23" s="22"/>
       <c r="G23" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" s="33" t="s">
         <v>70</v>
-      </c>
-      <c r="H23" s="33" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -4523,17 +5100,17 @@
         <v>4</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
       <c r="F24" s="22"/>
       <c r="G24" s="32" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H24" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" ht="24" spans="1:8">
@@ -4541,17 +5118,17 @@
         <v>5</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
       <c r="F25" s="22"/>
       <c r="G25" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25" s="33" t="s">
         <v>65</v>
-      </c>
-      <c r="H25" s="33" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="26" ht="24" spans="1:8">
@@ -4559,17 +5136,17 @@
         <v>6</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
       <c r="F26" s="22"/>
       <c r="G26" s="32" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H26" s="33" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -4577,7 +5154,7 @@
         <v>7</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
@@ -4587,7 +5164,7 @@
         <v>14</v>
       </c>
       <c r="H27" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" ht="24" spans="1:8">
@@ -4595,7 +5172,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="38" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C28" s="36"/>
       <c r="D28" s="36"/>
@@ -4605,7 +5182,7 @@
         <v>18</v>
       </c>
       <c r="H28" s="33" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -4691,7 +5268,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4703,33 +5280,33 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="7" t="s">
@@ -4739,7 +5316,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -4751,15 +5328,15 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="11"/>
       <c r="E6" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="14">
@@ -4769,15 +5346,15 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="16" t="s">
@@ -4787,7 +5364,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>18</v>
@@ -4801,10 +5378,10 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -4815,7 +5392,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -4824,7 +5401,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -4832,7 +5409,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
@@ -4840,7 +5417,7 @@
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
       <c r="H11" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -4848,7 +5425,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
@@ -4856,7 +5433,7 @@
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
       <c r="H12" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -4864,7 +5441,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
@@ -4872,7 +5449,7 @@
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
       <c r="H13" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -4880,7 +5457,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -4888,7 +5465,7 @@
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
       <c r="H14" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -4896,7 +5473,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
@@ -4904,7 +5481,7 @@
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
       <c r="H15" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -4912,7 +5489,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="21"/>
@@ -4920,7 +5497,7 @@
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
       <c r="H16" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -4961,7 +5538,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -4969,10 +5546,10 @@
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -4980,7 +5557,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
@@ -4990,7 +5567,7 @@
         <v>14</v>
       </c>
       <c r="H21" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -4998,17 +5575,17 @@
         <v>2</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="30"/>
       <c r="E22" s="30"/>
       <c r="F22" s="31"/>
       <c r="G22" s="32" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H22" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -5016,17 +5593,17 @@
         <v>3</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
       <c r="F23" s="22"/>
       <c r="G23" s="32" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H23" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -5034,7 +5611,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
@@ -5044,7 +5621,7 @@
         <v>18</v>
       </c>
       <c r="H24" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -5052,17 +5629,17 @@
         <v>5</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
       <c r="F25" s="22"/>
       <c r="G25" s="32" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H25" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -5070,17 +5647,17 @@
         <v>6</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
       <c r="F26" s="22"/>
       <c r="G26" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H26" s="33" t="s">
         <v>70</v>
-      </c>
-      <c r="H26" s="33" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -5088,17 +5665,17 @@
         <v>7</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
       <c r="F27" s="29"/>
       <c r="G27" s="32" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H27" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -5106,17 +5683,17 @@
         <v>8</v>
       </c>
       <c r="B28" s="35" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C28" s="36"/>
       <c r="D28" s="36"/>
       <c r="E28" s="36"/>
       <c r="F28" s="37"/>
       <c r="G28" s="32" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H28" s="34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -5202,7 +5779,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -5214,33 +5791,33 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="7" t="s">
@@ -5250,7 +5827,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -5262,15 +5839,15 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="11"/>
       <c r="E6" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="14">
@@ -5280,15 +5857,15 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="16" t="s">
@@ -5298,7 +5875,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>18</v>
@@ -5312,10 +5889,10 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -5326,7 +5903,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -5335,7 +5912,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -5343,7 +5920,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
@@ -5351,7 +5928,7 @@
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
       <c r="H11" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -5359,7 +5936,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
@@ -5367,7 +5944,7 @@
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
       <c r="H12" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -5375,7 +5952,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
@@ -5383,7 +5960,7 @@
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
       <c r="H13" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -5460,7 +6037,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -5468,10 +6045,10 @@
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -5479,17 +6056,17 @@
         <v>1</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
       <c r="E21" s="30"/>
       <c r="F21" s="31"/>
       <c r="G21" s="32" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H21" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -5497,17 +6074,17 @@
         <v>2</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="30"/>
       <c r="E22" s="30"/>
       <c r="F22" s="31"/>
       <c r="G22" s="32" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H22" s="34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -5515,17 +6092,17 @@
         <v>3</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
       <c r="F23" s="22"/>
       <c r="G23" s="32" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H23" s="34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -5533,17 +6110,17 @@
         <v>4</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
       <c r="F24" s="22"/>
       <c r="G24" s="32" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H24" s="34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -5551,7 +6128,7 @@
         <v>5</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
@@ -5561,7 +6138,7 @@
         <v>18</v>
       </c>
       <c r="H25" s="34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -5569,7 +6146,7 @@
         <v>6</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
@@ -5579,7 +6156,7 @@
         <v>14</v>
       </c>
       <c r="H26" s="34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -5587,17 +6164,17 @@
         <v>7</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
       <c r="F27" s="29"/>
       <c r="G27" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="33" t="s">
         <v>70</v>
-      </c>
-      <c r="H27" s="33" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -5605,17 +6182,17 @@
         <v>8</v>
       </c>
       <c r="B28" s="35" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C28" s="36"/>
       <c r="D28" s="36"/>
       <c r="E28" s="36"/>
       <c r="F28" s="37"/>
       <c r="G28" s="32" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H28" s="34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -5682,7 +6259,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:F27"/>
+      <selection activeCell="I29" sqref="A1:I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -5701,7 +6278,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -5713,33 +6290,33 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="7" t="s">
@@ -5749,7 +6326,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -5761,15 +6338,15 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="11"/>
       <c r="E6" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="14">
@@ -5779,15 +6356,15 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="16" t="s">
@@ -5797,7 +6374,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>18</v>
@@ -5811,10 +6388,10 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -5825,7 +6402,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -5834,7 +6411,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -5842,7 +6419,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
@@ -5850,7 +6427,7 @@
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
       <c r="H11" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -5858,7 +6435,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
@@ -5866,7 +6443,7 @@
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
       <c r="H12" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -5874,7 +6451,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
@@ -5882,7 +6459,7 @@
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
       <c r="H13" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -5890,7 +6467,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -5898,7 +6475,7 @@
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
       <c r="H14" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -5963,7 +6540,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
@@ -5971,10 +6548,10 @@
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -5982,17 +6559,17 @@
         <v>1</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
       <c r="E21" s="30"/>
       <c r="F21" s="31"/>
       <c r="G21" s="32" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H21" s="33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -6000,17 +6577,17 @@
         <v>2</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="30"/>
       <c r="E22" s="30"/>
       <c r="F22" s="31"/>
       <c r="G22" s="32" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H22" s="34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -6018,17 +6595,17 @@
         <v>3</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
       <c r="F23" s="22"/>
       <c r="G23" s="32" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H23" s="34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -6036,17 +6613,17 @@
         <v>4</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
       <c r="F24" s="22"/>
       <c r="G24" s="32" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H24" s="34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -6054,7 +6631,7 @@
         <v>5</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
@@ -6064,7 +6641,7 @@
         <v>18</v>
       </c>
       <c r="H25" s="34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -6072,7 +6649,7 @@
         <v>6</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
@@ -6082,7 +6659,7 @@
         <v>14</v>
       </c>
       <c r="H26" s="34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -6090,17 +6667,17 @@
         <v>7</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
       <c r="F27" s="29"/>
       <c r="G27" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="33" t="s">
         <v>70</v>
-      </c>
-      <c r="H27" s="33" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -6108,17 +6685,17 @@
         <v>8</v>
       </c>
       <c r="B28" s="35" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C28" s="36"/>
       <c r="D28" s="36"/>
       <c r="E28" s="36"/>
       <c r="F28" s="37"/>
       <c r="G28" s="32" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H28" s="34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>